<commit_message>
Refactored matchmaking algorithm. Also added command line arguments and headers for the excel file.
</commit_message>
<xml_diff>
--- a/data/mentors-clean.xlsx
+++ b/data/mentors-clean.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luisarojas/GDrive/Graduate/Winter2018/CSCI5020G_Collaborative_Design_and_Research/repo/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -943,8 +948,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1007,6 +1012,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1053,7 +1066,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1085,9 +1098,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1119,6 +1150,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1294,14 +1343,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1393,7 +1444,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1485,7 +1536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1577,7 +1628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1669,7 +1720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1761,7 +1812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1853,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1945,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -2037,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -2129,7 +2180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -2221,7 +2272,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -2313,7 +2364,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -2405,7 +2456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -2497,7 +2548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -2589,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2681,7 +2732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -2773,7 +2824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -2865,7 +2916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -2957,7 +3008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -3049,7 +3100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -3141,7 +3192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -3233,7 +3284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -3325,7 +3376,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -3417,7 +3468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -3509,7 +3560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -3601,7 +3652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -3693,7 +3744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -3785,7 +3836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -3877,7 +3928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -3969,7 +4020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -4061,7 +4112,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -4153,7 +4204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -4245,7 +4296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:30">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -4337,7 +4388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:30">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -4429,7 +4480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:30">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>60</v>
       </c>
@@ -4521,7 +4572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:30">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -4613,7 +4664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:30">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>61</v>
       </c>
@@ -4705,7 +4756,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:30">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -4797,7 +4848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:30">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -4889,7 +4940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:30">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>64</v>
       </c>
@@ -4981,7 +5032,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:30">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>65</v>
       </c>
@@ -5073,7 +5124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:30">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>66</v>
       </c>
@@ -5165,7 +5216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:30">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -5257,7 +5308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:30">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -5349,7 +5400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:30">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>68</v>
       </c>
@@ -5441,7 +5492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:30">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>69</v>
       </c>
@@ -5533,7 +5584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:30">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>70</v>
       </c>
@@ -5625,7 +5676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:30">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>71</v>
       </c>
@@ -5717,7 +5768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:30">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>72</v>
       </c>
@@ -5809,7 +5860,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:30">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>73</v>
       </c>
@@ -5901,7 +5952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:30">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>74</v>
       </c>
@@ -5993,7 +6044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:30">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>75</v>
       </c>
@@ -6085,7 +6136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:30">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>76</v>
       </c>
@@ -6177,7 +6228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:30">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>77</v>
       </c>
@@ -6269,7 +6320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:30">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>78</v>
       </c>
@@ -6361,7 +6412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:30">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>79</v>
       </c>
@@ -6453,7 +6504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:30">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>80</v>
       </c>
@@ -6545,7 +6596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:30">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>81</v>
       </c>
@@ -6637,7 +6688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:30">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -6729,7 +6780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:30">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>82</v>
       </c>
@@ -6821,7 +6872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:30">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>83</v>
       </c>
@@ -6913,7 +6964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:30">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>84</v>
       </c>
@@ -7005,7 +7056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:30">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>85</v>
       </c>
@@ -7097,7 +7148,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:30">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>86</v>
       </c>
@@ -7189,7 +7240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:30">
+    <row r="65" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>30</v>
       </c>
@@ -7281,7 +7332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:30">
+    <row r="66" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>41</v>
       </c>
@@ -7373,7 +7424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:30">
+    <row r="67" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>87</v>
       </c>
@@ -7465,7 +7516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:30">
+    <row r="68" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>88</v>
       </c>
@@ -7557,7 +7608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:30">
+    <row r="69" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>89</v>
       </c>
@@ -7649,7 +7700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:30">
+    <row r="70" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>90</v>
       </c>
@@ -7741,7 +7792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:30">
+    <row r="71" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>91</v>
       </c>
@@ -7833,7 +7884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:30">
+    <row r="72" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>92</v>
       </c>
@@ -7925,7 +7976,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:30">
+    <row r="73" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>93</v>
       </c>
@@ -8017,7 +8068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:30">
+    <row r="74" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>94</v>
       </c>
@@ -8109,7 +8160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:30">
+    <row r="75" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>95</v>
       </c>
@@ -8201,7 +8252,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:30">
+    <row r="76" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>96</v>
       </c>
@@ -8293,7 +8344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:30">
+    <row r="77" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>97</v>
       </c>
@@ -8385,7 +8436,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:30">
+    <row r="78" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>98</v>
       </c>
@@ -8477,7 +8528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:30">
+    <row r="79" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>99</v>
       </c>
@@ -8569,7 +8620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:30">
+    <row r="80" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>35</v>
       </c>
@@ -8661,7 +8712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:30">
+    <row r="81" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>100</v>
       </c>
@@ -8753,7 +8804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:30">
+    <row r="82" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>101</v>
       </c>
@@ -8845,7 +8896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:30">
+    <row r="83" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>102</v>
       </c>
@@ -8937,7 +8988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:30">
+    <row r="84" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>103</v>
       </c>
@@ -9029,7 +9080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:30">
+    <row r="85" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>104</v>
       </c>
@@ -9121,7 +9172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:30">
+    <row r="86" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>105</v>
       </c>
@@ -9213,7 +9264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:30">
+    <row r="87" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>106</v>
       </c>
@@ -9305,7 +9356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:30">
+    <row r="88" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>107</v>
       </c>
@@ -9397,7 +9448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:30">
+    <row r="89" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>108</v>
       </c>
@@ -9489,7 +9540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:30">
+    <row r="90" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>109</v>
       </c>
@@ -9581,7 +9632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:30">
+    <row r="91" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>110</v>
       </c>
@@ -9673,7 +9724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:30">
+    <row r="92" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>111</v>
       </c>
@@ -9765,7 +9816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:30">
+    <row r="93" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>112</v>
       </c>
@@ -9857,7 +9908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:30">
+    <row r="94" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>113</v>
       </c>
@@ -9949,7 +10000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:30">
+    <row r="95" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>114</v>
       </c>
@@ -10041,7 +10092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:30">
+    <row r="96" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>115</v>
       </c>
@@ -10133,7 +10184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:30">
+    <row r="97" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>116</v>
       </c>
@@ -10225,7 +10276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:30">
+    <row r="98" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>117</v>
       </c>
@@ -10317,7 +10368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:30">
+    <row r="99" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>118</v>
       </c>
@@ -10409,7 +10460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:30">
+    <row r="100" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>119</v>
       </c>
@@ -10501,7 +10552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:30">
+    <row r="101" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>120</v>
       </c>
@@ -10593,7 +10644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:30">
+    <row r="102" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>121</v>
       </c>
@@ -10685,7 +10736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:30">
+    <row r="103" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>122</v>
       </c>
@@ -10777,7 +10828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:30">
+    <row r="104" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>123</v>
       </c>
@@ -10869,7 +10920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:30">
+    <row r="105" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>39</v>
       </c>
@@ -10961,7 +11012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:30">
+    <row r="106" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>124</v>
       </c>
@@ -11053,7 +11104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:30">
+    <row r="107" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>30</v>
       </c>
@@ -11145,7 +11196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:30">
+    <row r="108" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>125</v>
       </c>
@@ -11237,7 +11288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:30">
+    <row r="109" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>59</v>
       </c>
@@ -11329,7 +11380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:30">
+    <row r="110" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>106</v>
       </c>

</xml_diff>